<commit_message>
Actualizacion del plan de metricas
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Medicion y Monitoreo/Plan Métricas-2015.xlsx
+++ b/qualtcom/Organizacional/Medicion y Monitoreo/Plan Métricas-2015.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\qtp\qualtcom\Organizacional\Medicion y Monitoreo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\qtp\qualtcom\Organizacional\Medicion y Monitoreo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-1365" yWindow="300" windowWidth="16605" windowHeight="9435" tabRatio="971" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="-1365" yWindow="300" windowWidth="16605" windowHeight="9435" tabRatio="971" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Objetivos de Medición" sheetId="1" r:id="rId1"/>
@@ -183,9 +183,6 @@
     <t>Reunión de reporte de monitoreo</t>
   </si>
   <si>
-    <t>Porcentaje de apego a productos=(Preguntas aprobadas+ preguntas que no aplican)/total de preguntas por fase</t>
-  </si>
-  <si>
     <t>Reunion de reporte de monitoreo</t>
   </si>
   <si>
@@ -460,6 +457,9 @@
   </si>
   <si>
     <t>Que el índice de satisfacción sea menor que 85% y mayor o igual a 70%</t>
+  </si>
+  <si>
+    <t>Porcentaje de apego a productos=(Preguntas aprobadas+ preguntas que no aplican)/total de preguntas por producto</t>
   </si>
 </sst>
 </file>
@@ -935,15 +935,6 @@
     <xf numFmtId="0" fontId="15" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -965,6 +956,15 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1401,11 +1401,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1326370080"/>
-        <c:axId val="-1326369536"/>
+        <c:axId val="104170896"/>
+        <c:axId val="104171456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1326370080"/>
+        <c:axId val="104170896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1415,7 +1415,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1326369536"/>
+        <c:crossAx val="104171456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1423,7 +1423,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1326369536"/>
+        <c:axId val="104171456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1437,7 +1437,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1326370080"/>
+        <c:crossAx val="104170896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1773,11 +1773,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1326364640"/>
-        <c:axId val="-1326367904"/>
+        <c:axId val="104176496"/>
+        <c:axId val="104177056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1326364640"/>
+        <c:axId val="104176496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1787,7 +1787,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1326367904"/>
+        <c:crossAx val="104177056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1795,7 +1795,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1326367904"/>
+        <c:axId val="104177056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1809,7 +1809,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1326364640"/>
+        <c:crossAx val="104176496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2141,11 +2141,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1327307664"/>
-        <c:axId val="-1327308208"/>
+        <c:axId val="103547856"/>
+        <c:axId val="103548416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1327307664"/>
+        <c:axId val="103547856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2155,7 +2155,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1327308208"/>
+        <c:crossAx val="103548416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2163,7 +2163,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1327308208"/>
+        <c:axId val="103548416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2177,7 +2177,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1327307664"/>
+        <c:crossAx val="103547856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2509,11 +2509,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1327306576"/>
-        <c:axId val="-1327303856"/>
+        <c:axId val="103979456"/>
+        <c:axId val="103980016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1327306576"/>
+        <c:axId val="103979456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2523,7 +2523,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1327303856"/>
+        <c:crossAx val="103980016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2531,7 +2531,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1327303856"/>
+        <c:axId val="103980016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2545,7 +2545,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1327306576"/>
+        <c:crossAx val="103979456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2877,11 +2877,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1327302768"/>
-        <c:axId val="-1327304400"/>
+        <c:axId val="103984496"/>
+        <c:axId val="103985056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1327302768"/>
+        <c:axId val="103984496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2891,7 +2891,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1327304400"/>
+        <c:crossAx val="103985056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2899,7 +2899,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1327304400"/>
+        <c:axId val="103985056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2913,7 +2913,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1327302768"/>
+        <c:crossAx val="103984496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3245,11 +3245,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1328040160"/>
-        <c:axId val="-1328039616"/>
+        <c:axId val="102846288"/>
+        <c:axId val="102846848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1328040160"/>
+        <c:axId val="102846288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3259,7 +3259,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1328039616"/>
+        <c:crossAx val="102846848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3267,7 +3267,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1328039616"/>
+        <c:axId val="102846848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3281,7 +3281,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1328040160"/>
+        <c:crossAx val="102846288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4252,13 +4252,13 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="18.75">
       <c r="A1" s="21"/>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
       <c r="G1" s="21"/>
     </row>
     <row r="2" spans="1:7">
@@ -4270,22 +4270,22 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="24.6" customHeight="1">
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="62" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="11" customFormat="1" ht="21" customHeight="1">
+      <c r="B4" s="62"/>
+      <c r="C4" s="23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="B5" s="62" t="s">
         <v>109</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="11" customFormat="1" ht="21" customHeight="1">
-      <c r="B4" s="54"/>
-      <c r="C4" s="23" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="B5" s="54" t="s">
-        <v>110</v>
       </c>
       <c r="C5" s="23" t="s">
         <v>22</v>
@@ -4294,32 +4294,32 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="22"/>
-      <c r="B6" s="54"/>
+      <c r="B6" s="62"/>
       <c r="C6" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="22"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="B7" s="62"/>
+      <c r="C7" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="22"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="B8" s="62"/>
+      <c r="C8" s="23" t="s">
         <v>88</v>
-      </c>
-      <c r="D6" s="22"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="B7" s="54"/>
-      <c r="C7" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="D7" s="22"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="B8" s="54"/>
-      <c r="C8" s="23" t="s">
-        <v>89</v>
       </c>
       <c r="D8" s="22"/>
     </row>
     <row r="9" spans="1:7" ht="30">
       <c r="B9" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -4328,13 +4328,13 @@
     </row>
     <row r="11" spans="1:7" s="2" customFormat="1" ht="18.75">
       <c r="A11" s="21"/>
-      <c r="B11" s="61" t="s">
+      <c r="B11" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="62"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="63"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="60"/>
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7" s="5" customFormat="1">
@@ -4342,55 +4342,55 @@
       <c r="B12" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="55" t="s">
+      <c r="C12" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="55"/>
-      <c r="E12" s="55" t="s">
+      <c r="D12" s="63"/>
+      <c r="E12" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="55"/>
+      <c r="F12" s="63"/>
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" s="5" customFormat="1">
       <c r="A13" s="3"/>
       <c r="B13" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="58" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="58"/>
-      <c r="E13" s="59" t="s">
-        <v>98</v>
-      </c>
-      <c r="F13" s="60"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="56" t="s">
+        <v>97</v>
+      </c>
+      <c r="F13" s="57"/>
     </row>
     <row r="14" spans="1:7" s="5" customFormat="1" ht="19.149999999999999" customHeight="1">
       <c r="A14" s="3"/>
       <c r="B14" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="56" t="s">
-        <v>90</v>
-      </c>
-      <c r="D14" s="57"/>
-      <c r="E14" s="59" t="s">
-        <v>99</v>
-      </c>
-      <c r="F14" s="60"/>
+        <v>55</v>
+      </c>
+      <c r="C14" s="53" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="54"/>
+      <c r="E14" s="56" t="s">
+        <v>98</v>
+      </c>
+      <c r="F14" s="57"/>
     </row>
     <row r="15" spans="1:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A15" s="3"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="58"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:7" s="5" customFormat="1" ht="26.25" customHeight="1">
       <c r="A16" s="3"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="55"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
     </row>
@@ -4413,16 +4413,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
     <mergeCell ref="C14:D16"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4471,15 +4471,15 @@
         <v>3</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="2:3" outlineLevel="1">
       <c r="B3" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="2:3" outlineLevel="1">
@@ -4511,7 +4511,7 @@
         <v>24</v>
       </c>
       <c r="C8" s="69" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="2:3" outlineLevel="1">
@@ -4522,10 +4522,10 @@
     </row>
     <row r="10" spans="2:3" outlineLevel="1">
       <c r="B10" s="30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="2:3" outlineLevel="1">
@@ -4536,7 +4536,7 @@
     </row>
     <row r="12" spans="2:3" ht="60" customHeight="1" outlineLevel="1">
       <c r="B12" s="65" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C12" s="65"/>
     </row>
@@ -4550,10 +4550,10 @@
     </row>
     <row r="14" spans="2:3" outlineLevel="1">
       <c r="B14" s="30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="2:3" outlineLevel="1">
@@ -4572,7 +4572,7 @@
     </row>
     <row r="17" spans="2:3" outlineLevel="1">
       <c r="B17" s="30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C17" s="32" t="s">
         <v>21</v>
@@ -4580,54 +4580,54 @@
     </row>
     <row r="18" spans="2:3" outlineLevel="1">
       <c r="B18" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="29" t="s">
         <v>74</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="19" spans="2:3" outlineLevel="1">
       <c r="B19" s="30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="2:3" outlineLevel="1">
       <c r="B20" s="66" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C20" s="66"/>
     </row>
     <row r="21" spans="2:3" s="18" customFormat="1" outlineLevel="1">
       <c r="B21" s="64" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C21" s="64"/>
     </row>
     <row r="22" spans="2:3" outlineLevel="1">
       <c r="B22" s="33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="30">
       <c r="B23" s="34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="30">
       <c r="B24" s="35" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="27:30">
@@ -4838,7 +4838,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="2:3" outlineLevel="1">
@@ -4846,7 +4846,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="2:3" outlineLevel="1">
@@ -4878,7 +4878,7 @@
         <v>36</v>
       </c>
       <c r="C8" s="69" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="2:3" outlineLevel="1">
@@ -4889,10 +4889,10 @@
     </row>
     <row r="10" spans="2:3" outlineLevel="1">
       <c r="B10" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" s="31" t="s">
         <v>104</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="11" spans="2:3" outlineLevel="1">
@@ -4903,7 +4903,7 @@
     </row>
     <row r="12" spans="2:3" ht="74.45" customHeight="1" outlineLevel="1">
       <c r="B12" s="65" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C12" s="65"/>
     </row>
@@ -4917,10 +4917,10 @@
     </row>
     <row r="14" spans="2:3" outlineLevel="1">
       <c r="B14" s="30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="2:3" outlineLevel="1">
@@ -4939,7 +4939,7 @@
     </row>
     <row r="17" spans="2:3" outlineLevel="1">
       <c r="B17" s="30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C17" s="32" t="s">
         <v>21</v>
@@ -4947,48 +4947,48 @@
     </row>
     <row r="18" spans="2:3" outlineLevel="1">
       <c r="B18" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="29" t="s">
         <v>74</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="19" spans="2:3" outlineLevel="1">
       <c r="B19" s="30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="2:3" outlineLevel="1">
       <c r="B20" s="66" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C20" s="66"/>
     </row>
     <row r="21" spans="2:3" outlineLevel="1">
       <c r="B21" s="33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="30">
       <c r="B22" s="34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="30">
       <c r="B23" s="35" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="27:30">
@@ -5168,8 +5168,8 @@
   </sheetPr>
   <dimension ref="B1:AD47"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -5198,15 +5198,15 @@
         <v>3</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="13.15" customHeight="1" outlineLevel="1">
       <c r="B3" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="2:3" outlineLevel="1">
@@ -5261,7 +5261,7 @@
     </row>
     <row r="12" spans="2:3" ht="77.25" customHeight="1" outlineLevel="1">
       <c r="B12" s="65" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C12" s="65"/>
     </row>
@@ -5275,7 +5275,7 @@
     </row>
     <row r="14" spans="2:3" outlineLevel="1">
       <c r="B14" s="30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C14" s="30" t="s">
         <v>39</v>
@@ -5297,7 +5297,7 @@
     </row>
     <row r="17" spans="2:3" outlineLevel="1">
       <c r="B17" s="30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C17" s="32" t="s">
         <v>49</v>
@@ -5305,10 +5305,10 @@
     </row>
     <row r="18" spans="2:3" outlineLevel="1">
       <c r="B18" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="29" t="s">
         <v>74</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="19" spans="2:3" outlineLevel="1">
@@ -5316,12 +5316,12 @@
         <v>39</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="2:3" outlineLevel="1">
       <c r="B20" s="66" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C20" s="66"/>
     </row>
@@ -5330,7 +5330,7 @@
         <v>46</v>
       </c>
       <c r="C21" s="40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="2:3">
@@ -5338,7 +5338,7 @@
         <v>47</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="2:3">
@@ -5346,7 +5346,7 @@
         <v>48</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="27:30">
@@ -5526,8 +5526,8 @@
   </sheetPr>
   <dimension ref="B1:AD47"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:C6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -5556,15 +5556,15 @@
         <v>3</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="2:3" outlineLevel="1">
       <c r="B3" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="2:3" outlineLevel="1">
@@ -5596,7 +5596,7 @@
         <v>42</v>
       </c>
       <c r="C8" s="70" t="s">
-        <v>50</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="2:3" outlineLevel="1">
@@ -5619,7 +5619,7 @@
     </row>
     <row r="12" spans="2:3" ht="73.150000000000006" customHeight="1" outlineLevel="1">
       <c r="B12" s="65" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C12" s="65"/>
     </row>
@@ -5633,7 +5633,7 @@
     </row>
     <row r="14" spans="2:3" outlineLevel="1">
       <c r="B14" s="30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C14" s="30" t="s">
         <v>39</v>
@@ -5655,18 +5655,18 @@
     </row>
     <row r="17" spans="2:3" outlineLevel="1">
       <c r="B17" s="30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="2:3" outlineLevel="1">
       <c r="B18" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="29" t="s">
         <v>74</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="19" spans="2:3" outlineLevel="1">
@@ -5674,12 +5674,12 @@
         <v>39</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="2:3" outlineLevel="1">
       <c r="B20" s="66" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C20" s="66"/>
     </row>
@@ -5688,7 +5688,7 @@
         <v>46</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="2:3">
@@ -5696,7 +5696,7 @@
         <v>47</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="2:3">
@@ -5704,7 +5704,7 @@
         <v>48</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="27:30">
@@ -5914,15 +5914,15 @@
         <v>3</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="2:3" outlineLevel="1">
       <c r="B3" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="2:3" outlineLevel="1">
@@ -5954,7 +5954,7 @@
         <v>42</v>
       </c>
       <c r="C8" s="70" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="2:3" outlineLevel="1">
@@ -5977,7 +5977,7 @@
     </row>
     <row r="12" spans="2:3" ht="46.9" customHeight="1" outlineLevel="1">
       <c r="B12" s="65" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C12" s="65"/>
     </row>
@@ -5991,7 +5991,7 @@
     </row>
     <row r="14" spans="2:3" outlineLevel="1">
       <c r="B14" s="30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C14" s="30" t="s">
         <v>39</v>
@@ -6013,18 +6013,18 @@
     </row>
     <row r="17" spans="2:3" outlineLevel="1">
       <c r="B17" s="30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="2:3" outlineLevel="1">
       <c r="B18" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="29" t="s">
         <v>74</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="19" spans="2:3" outlineLevel="1">
@@ -6032,12 +6032,12 @@
         <v>39</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="2:3" outlineLevel="1">
       <c r="B20" s="66" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C20" s="66"/>
     </row>
@@ -6046,7 +6046,7 @@
         <v>46</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="2:3">
@@ -6054,7 +6054,7 @@
         <v>47</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="2:3">
@@ -6062,7 +6062,7 @@
         <v>48</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="27:30">
@@ -6312,7 +6312,7 @@
         <v>42</v>
       </c>
       <c r="C8" s="70" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="2:3" outlineLevel="1">
@@ -6335,7 +6335,7 @@
     </row>
     <row r="12" spans="2:3" ht="45.6" customHeight="1" outlineLevel="1">
       <c r="B12" s="65" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C12" s="65"/>
     </row>
@@ -6349,7 +6349,7 @@
     </row>
     <row r="14" spans="2:3" outlineLevel="1">
       <c r="B14" s="30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C14" s="30" t="s">
         <v>39</v>
@@ -6371,31 +6371,31 @@
     </row>
     <row r="17" spans="2:3" outlineLevel="1">
       <c r="B17" s="30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="2:3" outlineLevel="1">
       <c r="B18" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="29" t="s">
         <v>74</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="19" spans="2:3" outlineLevel="1">
       <c r="B19" s="30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="2:3" outlineLevel="1">
       <c r="B20" s="66" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C20" s="66"/>
     </row>
@@ -6404,7 +6404,7 @@
         <v>46</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="2:3">
@@ -6412,7 +6412,7 @@
         <v>47</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="2:3">
@@ -6420,7 +6420,7 @@
         <v>48</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="27:30">
@@ -6598,7 +6598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -6623,7 +6623,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -6631,7 +6631,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -6650,19 +6650,19 @@
       </c>
       <c r="B6" s="72"/>
       <c r="Q6" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="R6" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="R6" s="11" t="s">
+      <c r="S6" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="S6" s="11" t="s">
+      <c r="T6" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="T6" s="11" t="s">
+      <c r="U6" s="11" t="s">
         <v>62</v>
-      </c>
-      <c r="U6" s="11" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -6670,10 +6670,10 @@
         <v>20</v>
       </c>
       <c r="B7" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="P7" s="11" t="s">
         <v>64</v>
-      </c>
-      <c r="P7" s="11" t="s">
-        <v>65</v>
       </c>
       <c r="Q7" s="11">
         <f>AVERAGE(R7:U7)</f>
@@ -6694,13 +6694,13 @@
     </row>
     <row r="8" spans="1:21" ht="30">
       <c r="A8" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="P8" s="11" t="s">
         <v>67</v>
-      </c>
-      <c r="P8" s="11" t="s">
-        <v>68</v>
       </c>
       <c r="Q8" s="11">
         <f>AVERAGE(R8:U8)</f>
@@ -6727,7 +6727,7 @@
     </row>
     <row r="10" spans="1:21" ht="61.5" customHeight="1">
       <c r="A10" s="75" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B10" s="75"/>
     </row>
@@ -6741,10 +6741,10 @@
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -6763,62 +6763,62 @@
     </row>
     <row r="15" spans="1:21">
       <c r="A15" s="30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="49" t="s">
         <v>69</v>
-      </c>
-      <c r="B16" s="49" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="72" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B18" s="72"/>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="71" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B19" s="71"/>
     </row>
     <row r="20" spans="1:2" ht="28.5">
       <c r="A20" s="50" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="30">
       <c r="A21" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="52" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>